<commit_message>
minor changes to Name class and subsequent functions
</commit_message>
<xml_diff>
--- a/samples/names_20210618_072058.xlsx
+++ b/samples/names_20210618_072058.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masayukikishi/Dropbox (Personal)/masayuki_kishi/repositories/create_names/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C0BBEF9-2C19-334D-8071-0FB8BF6BDDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E640BD-228E-6548-841E-A65DD12189BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,12 +64,6 @@
     <t>| Trees | Great |</t>
   </si>
   <si>
-    <t>Trees</t>
-  </si>
-  <si>
-    <t>Great</t>
-  </si>
-  <si>
     <t>LordtoJuly</t>
   </si>
   <si>
@@ -79,12 +73,6 @@
     <t>| Lord | July |</t>
   </si>
   <si>
-    <t>Lord</t>
-  </si>
-  <si>
-    <t>July</t>
-  </si>
-  <si>
     <t>noun + and + noun</t>
   </si>
   <si>
@@ -97,12 +85,6 @@
     <t>| Menu | Name |</t>
   </si>
   <si>
-    <t>Menu</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>LifetoGarden</t>
   </si>
   <si>
@@ -112,12 +94,6 @@
     <t>| Life | Garden |</t>
   </si>
   <si>
-    <t>Life</t>
-  </si>
-  <si>
-    <t>Garden</t>
-  </si>
-  <si>
     <t>LittoKingdom</t>
   </si>
   <si>
@@ -127,12 +103,6 @@
     <t>| Lit | Kingdom |</t>
   </si>
   <si>
-    <t>Lit</t>
-  </si>
-  <si>
-    <t>Kingdom</t>
-  </si>
-  <si>
     <t>PlanttoYear</t>
   </si>
   <si>
@@ -142,12 +112,6 @@
     <t>| Plant | Year |</t>
   </si>
   <si>
-    <t>Plant</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>MayandWorld</t>
   </si>
   <si>
@@ -157,12 +121,6 @@
     <t>| May | World |</t>
   </si>
   <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>World</t>
-  </si>
-  <si>
     <t>TreestoDon</t>
   </si>
   <si>
@@ -172,9 +130,6 @@
     <t>| Trees | Don |</t>
   </si>
   <si>
-    <t>Don</t>
-  </si>
-  <si>
     <t>AwardtoPlate</t>
   </si>
   <si>
@@ -184,12 +139,6 @@
     <t>| Award | Plate |</t>
   </si>
   <si>
-    <t>Award</t>
-  </si>
-  <si>
-    <t>Plate</t>
-  </si>
-  <si>
     <t>FossiltoJung</t>
   </si>
   <si>
@@ -199,16 +148,67 @@
     <t>| Fossil | Jung |</t>
   </si>
   <si>
-    <t>Fossil</t>
-  </si>
-  <si>
-    <t>Jung</t>
-  </si>
-  <si>
     <t>w</t>
   </si>
   <si>
     <t>b</t>
+  </si>
+  <si>
+    <t>['Trees','noun']</t>
+  </si>
+  <si>
+    <t>['Great','noun']</t>
+  </si>
+  <si>
+    <t>['Lord','noun']</t>
+  </si>
+  <si>
+    <t>['July','noun']</t>
+  </si>
+  <si>
+    <t>['Menu','noun']</t>
+  </si>
+  <si>
+    <t>['Name','noun']</t>
+  </si>
+  <si>
+    <t>['Life','noun']</t>
+  </si>
+  <si>
+    <t>['Garden','noun']</t>
+  </si>
+  <si>
+    <t>['Lit','noun']</t>
+  </si>
+  <si>
+    <t>['Kingdom','noun']</t>
+  </si>
+  <si>
+    <t>['Plant','noun']</t>
+  </si>
+  <si>
+    <t>['Year','noun']</t>
+  </si>
+  <si>
+    <t>['May','noun']</t>
+  </si>
+  <si>
+    <t>['World','noun']</t>
+  </si>
+  <si>
+    <t>['Don','noun']</t>
+  </si>
+  <si>
+    <t>['Award','noun']</t>
+  </si>
+  <si>
+    <t>['Plate','noun']</t>
+  </si>
+  <si>
+    <t>['Fossil','noun']</t>
+  </si>
+  <si>
+    <t>['Jung','noun']</t>
   </si>
 </sst>
 </file>
@@ -575,10 +575,15 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="183" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
@@ -632,10 +637,10 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -649,22 +654,22 @@
         <v>10</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -672,28 +677,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="K4" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -707,25 +712,25 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -739,25 +744,25 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="I6" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -771,19 +776,19 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H7" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -791,25 +796,25 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C8">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H8" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -823,28 +828,28 @@
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -858,25 +863,25 @@
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I10" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -890,19 +895,19 @@
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>